<commit_message>
kashefipour and timindexer added, minor changes in main watum09 m file were made
</commit_message>
<xml_diff>
--- a/seo_paper_02.xlsx
+++ b/seo_paper_02.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
@@ -12,10 +12,10 @@
     <sheet name="Initial Concentration" sheetId="10" r:id="rId3"/>
     <sheet name="Loading" sheetId="3" r:id="rId4"/>
     <sheet name="hidden tab" sheetId="11" r:id="rId5"/>
-    <sheet name="LDC" sheetId="12" r:id="rId6"/>
-    <sheet name="چاتا" sheetId="14" r:id="rId7"/>
-    <sheet name="ماکیناو" sheetId="15" r:id="rId8"/>
-    <sheet name="سورن سفارش نوری" sheetId="13" r:id="rId9"/>
+    <sheet name="LDC" sheetId="12" state="hidden" r:id="rId6"/>
+    <sheet name="چاتا" sheetId="14" state="hidden" r:id="rId7"/>
+    <sheet name="ماکیناو" sheetId="15" state="hidden" r:id="rId8"/>
+    <sheet name="سورن سفارش نوری" sheetId="13" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Delta_T__seconds">Setting!$B$10</definedName>
@@ -370,9 +370,6 @@
     <t>Concentration (ppm)</t>
   </si>
   <si>
-    <t>paper_02</t>
-  </si>
-  <si>
     <t>Elder (1959)</t>
   </si>
   <si>
@@ -428,6 +425,9 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>paper_02_seo_</t>
   </si>
 </sst>
 </file>
@@ -1557,15 +1557,6 @@
     <xf numFmtId="11" fontId="0" fillId="32" borderId="7" xfId="37" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1577,6 +1568,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -4801,8 +4801,8 @@
   </sheetPr>
   <dimension ref="A1:X91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4843,7 +4843,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -7829,14 +7829,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="47.140625" style="85" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="47.140625" style="82" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -7846,8 +7846,8 @@
       <c r="H1">
         <v>1</v>
       </c>
-      <c r="N1" s="82" t="s">
-        <v>107</v>
+      <c r="N1" s="79" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -7857,8 +7857,8 @@
       <c r="H2">
         <v>5</v>
       </c>
-      <c r="N2" s="84" t="s">
-        <v>89</v>
+      <c r="N2" s="81" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -7868,8 +7868,8 @@
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="N3" s="84" t="s">
-        <v>90</v>
+      <c r="N3" s="81" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7879,8 +7879,8 @@
       <c r="H4">
         <v>25</v>
       </c>
-      <c r="N4" s="84" t="s">
-        <v>91</v>
+      <c r="N4" s="81" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -7890,8 +7890,8 @@
       <c r="H5">
         <v>50</v>
       </c>
-      <c r="N5" s="84" t="s">
-        <v>92</v>
+      <c r="N5" s="81" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -7901,8 +7901,8 @@
       <c r="H6">
         <v>100</v>
       </c>
-      <c r="N6" s="84" t="s">
-        <v>93</v>
+      <c r="N6" s="81" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -7912,8 +7912,8 @@
       <c r="H7">
         <v>150</v>
       </c>
-      <c r="N7" s="84" t="s">
-        <v>94</v>
+      <c r="N7" s="81" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -7923,8 +7923,8 @@
       <c r="H8">
         <v>200</v>
       </c>
-      <c r="N8" s="84" t="s">
-        <v>95</v>
+      <c r="N8" s="81" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -7934,8 +7934,8 @@
       <c r="H9">
         <v>250</v>
       </c>
-      <c r="N9" s="84" t="s">
-        <v>96</v>
+      <c r="N9" s="81" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -7945,87 +7945,87 @@
       <c r="H10">
         <v>300</v>
       </c>
-      <c r="N10" s="84" t="s">
-        <v>97</v>
+      <c r="N10" s="81" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H11">
         <v>350</v>
       </c>
-      <c r="N11" s="84" t="s">
-        <v>98</v>
+      <c r="N11" s="81" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H12">
         <v>400</v>
       </c>
-      <c r="N12" s="84" t="s">
-        <v>99</v>
+      <c r="N12" s="81" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H13">
         <v>450</v>
       </c>
-      <c r="N13" s="84" t="s">
-        <v>100</v>
+      <c r="N13" s="81" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H14">
         <v>500</v>
       </c>
-      <c r="N14" s="84" t="s">
-        <v>101</v>
+      <c r="N14" s="81" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H15">
         <v>550</v>
       </c>
-      <c r="N15" s="84" t="s">
-        <v>102</v>
+      <c r="N15" s="81" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H16">
         <v>600</v>
       </c>
-      <c r="N16" s="84" t="s">
-        <v>103</v>
+      <c r="N16" s="81" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H17">
         <v>650</v>
       </c>
-      <c r="N17" s="84" t="s">
-        <v>104</v>
+      <c r="N17" s="81" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H18">
         <v>700</v>
       </c>
-      <c r="N18" s="84" t="s">
-        <v>105</v>
+      <c r="N18" s="81" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H19">
         <v>750</v>
       </c>
-      <c r="N19" s="84" t="s">
-        <v>106</v>
+      <c r="N19" s="81" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H20">
         <v>800</v>
       </c>
-      <c r="N20" s="85" t="s">
+      <c r="N20" s="82" t="s">
         <v>8</v>
       </c>
     </row>
@@ -8043,7 +8043,7 @@
       <c r="H23">
         <v>1250</v>
       </c>
-      <c r="N23" s="83"/>
+      <c r="N23" s="80"/>
     </row>
     <row r="24" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H24">
@@ -8080,7 +8080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8994,15 +8994,15 @@
     </row>
     <row r="28" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="60"/>
-      <c r="G28" s="79" t="s">
+      <c r="G28" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="H28" s="80"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="80"/>
-      <c r="L28" s="80"/>
-      <c r="M28" s="81"/>
+      <c r="H28" s="84"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="84"/>
+      <c r="L28" s="84"/>
+      <c r="M28" s="85"/>
     </row>
     <row r="29" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="61" t="s">

</xml_diff>